<commit_message>
feat: Project Restructuring and CLI Enhancements
- Added Makefile and smoke tests
- Updated project structure with case_files/
- Refactored CLI to support --input and --open flags
- Updated documentation
- Added .gitignore and cleaned up build artifacts
</commit_message>
<xml_diff>
--- a/output/biometano/biometano_report.xlsx
+++ b/output/biometano/biometano_report.xlsx
@@ -1544,13 +1544,13 @@
         <v>75000</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>600000</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>222500</v>
+        <v>244000</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>150000</v>
@@ -1562,7 +1562,7 @@
         <v>37500</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>2995000</v>
+        <v>3102500</v>
       </c>
     </row>
     <row r="5">
@@ -1579,13 +1579,13 @@
         <v>91800</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>907800</v>
+        <v>995520</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>737999.9999999999</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>224725</v>
+        <v>246440</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>183600</v>
@@ -1597,7 +1597,7 @@
         <v>45900</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>3443725</v>
+        <v>3553160</v>
       </c>
     </row>
     <row r="6">
@@ -1614,13 +1614,13 @@
         <v>98838</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>925956</v>
+        <v>1015430.4</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>798474.9999999999</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>226972.25</v>
+        <v>248904.4</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>197676</v>
@@ -1632,7 +1632,7 @@
         <v>49419</v>
       </c>
       <c r="K6" s="3" t="n">
-        <v>3648933.55</v>
+        <v>3760340.1</v>
       </c>
     </row>
     <row r="7">
@@ -1649,13 +1649,13 @@
         <v>100814.76</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>944475.1200000001</v>
+        <v>1035739.008</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>818436.8749999998</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>229241.9725</v>
+        <v>251393.444</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>201629.52</v>
@@ -1667,7 +1667,7 @@
         <v>50407.38</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>3727464.7225</v>
+        <v>3840880.082</v>
       </c>
     </row>
     <row r="8">
@@ -1684,13 +1684,13 @@
         <v>102831.0552</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>963364.6224</v>
+        <v>1056453.78816</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>838897.7968749997</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>231534.392225</v>
+        <v>253907.37844</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>205662.1104</v>
@@ -1702,7 +1702,7 @@
         <v>51415.5276</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>3807758.52607</v>
+        <v>3923220.678045</v>
       </c>
     </row>
     <row r="9">
@@ -1719,13 +1719,13 @@
         <v>104887.676304</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>982631.914848</v>
+        <v>1077582.8639232</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>859870.2417968746</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>233849.73614725</v>
+        <v>256446.4522244</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>209775.352608</v>
@@ -1737,7 +1737,7 @@
         <v>52443.838152</v>
       </c>
       <c r="K9" s="3" t="n">
-        <v>3889855.928457625</v>
+        <v>4007403.593609975</v>
       </c>
     </row>
     <row r="10">
@@ -1754,13 +1754,13 @@
         <v>106985.42983008</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>1002284.55314496</v>
+        <v>1099134.521201664</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>881366.9978417964</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>236188.2335087225</v>
+        <v>259010.916746644</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>213970.85966016</v>
@@ -1772,7 +1772,7 @@
         <v>53492.71491504</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>3973798.880282512</v>
+        <v>4093471.531577137</v>
       </c>
     </row>
     <row r="11">
@@ -1789,13 +1789,13 @@
         <v>109125.1384266816</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>1022330.244207859</v>
+        <v>1121117.211625697</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>903401.1727878413</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>238550.1158438097</v>
+        <v>261601.0259141104</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>218250.2768533632</v>
@@ -1807,7 +1807,7 @@
         <v>54562.5692133408</v>
       </c>
       <c r="K11" s="3" t="n">
-        <v>4059630.339332754</v>
+        <v>4181468.216820892</v>
       </c>
     </row>
     <row r="12">
@@ -1824,13 +1824,13 @@
         <v>111307.6411952152</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>1042776.849092016</v>
+        <v>1143539.555858211</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>925986.2021075371</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>240935.6170022479</v>
+        <v>264217.0361732516</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>222615.2823904305</v>
@@ -1842,7 +1842,7 @@
         <v>55653.82059760762</v>
       </c>
       <c r="K12" s="3" t="n">
-        <v>4147394.295479094</v>
+        <v>4271438.421416292</v>
       </c>
     </row>
     <row r="13">
@@ -1859,13 +1859,13 @@
         <v>113533.7940191196</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>1063632.386073857</v>
+        <v>1166410.346975376</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>949135.8571602255</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>243344.9731722703</v>
+        <v>266859.2065349841</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>227067.5880382391</v>
@@ -1877,7 +1877,7 @@
         <v>56766.89700955978</v>
       </c>
       <c r="K13" s="3" t="n">
-        <v>4237135.796223</v>
+        <v>4363427.990487233</v>
       </c>
     </row>
     <row r="14">
@@ -1894,13 +1894,13 @@
         <v>115804.4698995019</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>1084905.033795334</v>
+        <v>1189738.553914883</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>972864.2535892309</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>245778.422903993</v>
+        <v>269527.7986003339</v>
       </c>
       <c r="H14" s="3" t="n">
         <v>231608.9397990039</v>
@@ -1912,7 +1912,7 @@
         <v>57902.23494975097</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>4328900.972895162</v>
+        <v>4457483.868711052</v>
       </c>
     </row>
     <row r="15">
@@ -1929,13 +1929,13 @@
         <v>118120.559297492</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>1106603.134471241</v>
+        <v>1213533.324993181</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>997185.8599289617</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>248236.2071330329</v>
+        <v>272223.0765863372</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>236241.118594984</v>
@@ -1947,7 +1947,7 @@
         <v>59060.27964874599</v>
       </c>
       <c r="K15" s="3" t="n">
-        <v>4422737.067521404</v>
+        <v>4553654.127496649</v>
       </c>
     </row>
     <row r="16">
@@ -1964,13 +1964,13 @@
         <v>120482.9704834418</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>1128735.197160665</v>
+        <v>1237803.991493044</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>1022115.506427186</v>
       </c>
       <c r="G16" s="3" t="n">
-        <v>250718.5692043633</v>
+        <v>274945.3073522006</v>
       </c>
       <c r="H16" s="3" t="n">
         <v>240965.9409668836</v>
@@ -1982,7 +1982,7 @@
         <v>60241.48524172091</v>
       </c>
       <c r="K16" s="3" t="n">
-        <v>4518692.46037346</v>
+        <v>4651987.992853677</v>
       </c>
     </row>
     <row r="17">
@@ -1999,13 +1999,13 @@
         <v>122892.6298931107</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>1151309.901103879</v>
+        <v>1262560.071322905</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>1047668.394087865</v>
       </c>
       <c r="G17" s="3" t="n">
-        <v>253225.7548964069</v>
+        <v>277694.7604257226</v>
       </c>
       <c r="H17" s="3" t="n">
         <v>245785.2597862213</v>
@@ -2017,7 +2017,7 @@
         <v>61446.31494655534</v>
       </c>
       <c r="K17" s="3" t="n">
-        <v>4616816.698222538</v>
+        <v>4752535.873970879</v>
       </c>
     </row>
     <row r="18">
@@ -2034,13 +2034,13 @@
         <v>125350.4824909729</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>1174336.099125956</v>
+        <v>1287811.272749363</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>1073860.103940062</v>
       </c>
       <c r="G18" s="3" t="n">
-        <v>255758.012445371</v>
+        <v>280471.7080299799</v>
       </c>
       <c r="H18" s="3" t="n">
         <v>250700.9649819458</v>
@@ -2052,7 +2052,7 @@
         <v>62675.24124548644</v>
       </c>
       <c r="K18" s="3" t="n">
-        <v>4717160.523314024</v>
+        <v>4855349.392522041</v>
       </c>
     </row>
     <row r="19">
@@ -2069,13 +2069,13 @@
         <v>127857.4921407923</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>1197822.821108476</v>
+        <v>1313567.498204351</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>1100706.606538563</v>
       </c>
       <c r="G19" s="3" t="n">
-        <v>258315.5925698247</v>
+        <v>283276.4251102797</v>
       </c>
       <c r="H19" s="3" t="n">
         <v>255714.9842815846</v>
@@ -2087,7 +2087,7 @@
         <v>63928.74607039616</v>
       </c>
       <c r="K19" s="3" t="n">
-        <v>4819775.903082277</v>
+        <v>4960481.412718607</v>
       </c>
     </row>
     <row r="20">
@@ -2104,13 +2104,13 @@
         <v>130414.6419836082</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>1221779.277530645</v>
+        <v>1339838.848168438</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>1128224.271702027</v>
       </c>
       <c r="G20" s="3" t="n">
-        <v>260898.748495523</v>
+        <v>286109.1893613825</v>
       </c>
       <c r="H20" s="3" t="n">
         <v>260829.2839672164</v>
@@ -2122,7 +2122,7 @@
         <v>65207.32099180409</v>
       </c>
       <c r="K20" s="3" t="n">
-        <v>4924716.060624847</v>
+        <v>5067986.072128499</v>
       </c>
     </row>
   </sheetData>
@@ -2150,9 +2150,9 @@
     <col width="20" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="19" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
     <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="19" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
     <col width="21" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
     <col width="20" customWidth="1" min="12" max="12"/>
@@ -2316,37 +2316,37 @@
         <v>11119755</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>2995000</v>
+        <v>3102500</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>8124755</v>
+        <v>8017255</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>6820572.174515235</v>
+        <v>6584109.83055134</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>1375000</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>5445572.174515235</v>
+        <v>5209109.83055134</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>1306937.321883656</v>
+        <v>1250186.359332322</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>1093337.321883656</v>
+        <v>1015946.359332322</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>213600</v>
+        <v>234240</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>5231972.174515235</v>
+        <v>4974869.83055134</v>
       </c>
     </row>
     <row r="5">
@@ -2357,37 +2357,37 @@
         <v>13354102.26</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>3443725</v>
+        <v>3553160</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>9910377.26</v>
+        <v>9800942.26</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>8606194.434515234</v>
+        <v>8367797.09055134</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>1250000</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>7356194.434515234</v>
+        <v>7117797.09055134</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>1765486.664283656</v>
+        <v>1708271.301732322</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>1551886.664283656</v>
+        <v>1474031.301732322</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>213599.9999999998</v>
+        <v>234240</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>7142594.434515234</v>
+        <v>6883557.09055134</v>
       </c>
     </row>
     <row r="6">
@@ -2398,37 +2398,37 @@
         <v>14107184.3663</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>3648933.55</v>
+        <v>3760340.1</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>10458250.8163</v>
+        <v>10346844.2663</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>9154067.990815237</v>
+        <v>8913699.096851341</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>1125000</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>8029067.990815237</v>
+        <v>7788699.096851341</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>1926976.317795657</v>
+        <v>1869287.783244322</v>
       </c>
       <c r="K6" s="3" t="n">
-        <v>1713376.317795657</v>
+        <v>1635047.783244322</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>213600.0000000002</v>
+        <v>234240.0000000002</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>7815467.990815237</v>
+        <v>7554459.096851341</v>
       </c>
     </row>
     <row r="7">
@@ -2439,37 +2439,37 @@
         <v>14118589.825323</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>3727464.7225</v>
+        <v>3840880.082</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>10391125.102823</v>
+        <v>10277709.743323</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>9086942.277338237</v>
+        <v>8844564.573874339</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>1000000</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>8086942.277338237</v>
+        <v>7844564.573874339</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>1940866.146561177</v>
+        <v>1882695.497729841</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>1727266.146561177</v>
+        <v>1648455.497729842</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>213600.0000000002</v>
+        <v>234239.9999999998</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>7873342.277338237</v>
+        <v>7610324.573874339</v>
       </c>
     </row>
     <row r="8">
@@ -2480,37 +2480,37 @@
         <v>14130217.50724343</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>3807758.52607</v>
+        <v>3923220.678045</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>10322458.98117343</v>
+        <v>10206996.82919843</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>9018276.155688666</v>
+        <v>8773851.659749769</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>875000</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>8143276.155688666</v>
+        <v>7898851.659749769</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>1954386.27736528</v>
+        <v>1895724.398339944</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>419544.0494758552</v>
+        <v>1360542.257961195</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>1534842.227889424</v>
+        <v>535182.140378749</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>6608433.927799242</v>
+        <v>7363669.51937102</v>
       </c>
     </row>
     <row r="9">
@@ -2521,37 +2521,37 @@
         <v>14142071.79765641</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>3889855.928457625</v>
+        <v>4007403.593609975</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>10252215.86919878</v>
+        <v>10134668.20404643</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>8948033.043714017</v>
+        <v>8701523.034597773</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>750000</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>8198033.043714017</v>
+        <v>7951523.034597773</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>1967527.930491364</v>
+        <v>1908365.528303466</v>
       </c>
       <c r="K9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>1967527.930491364</v>
+        <v>1908365.528303466</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>6230505.113222653</v>
+        <v>6043157.506294307</v>
       </c>
     </row>
     <row r="10">
@@ -2562,37 +2562,37 @@
         <v>14154157.16928033</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>3973798.880282512</v>
+        <v>4093471.531577137</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>10180358.28899781</v>
+        <v>10060685.63770319</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>8876175.46351305</v>
+        <v>8627540.468254529</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>625000</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>8251175.46351305</v>
+        <v>8002540.468254529</v>
       </c>
       <c r="J10" s="3" t="n">
-        <v>1980282.111243132</v>
+        <v>1920609.712381087</v>
       </c>
       <c r="K10" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>1980282.111243132</v>
+        <v>1920609.712381087</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>6270893.352269918</v>
+        <v>6081930.755873442</v>
       </c>
     </row>
     <row r="11">
@@ -2603,37 +2603,37 @@
         <v>14166478.18369343</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>4059630.339332754</v>
+        <v>4181468.216820892</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>10106847.84436068</v>
+        <v>9985009.966872541</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>8802665.018875916</v>
+        <v>8551864.797423881</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>500000</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>8302665.018875916</v>
+        <v>8051864.797423881</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>1992639.60453022</v>
+        <v>1932447.551381731</v>
       </c>
       <c r="K11" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>1992639.60453022</v>
+        <v>1932447.551381731</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>6310025.414345696</v>
+        <v>6119417.246042149</v>
       </c>
     </row>
     <row r="12">
@@ -2644,37 +2644,37 @@
         <v>14179039.49310508</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>4147394.295479094</v>
+        <v>4271438.421416292</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>10031645.19762598</v>
+        <v>9907601.071688784</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>8727462.37214122</v>
+        <v>8474455.902240124</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>375000</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>8352462.37214122</v>
+        <v>8099455.902240124</v>
       </c>
       <c r="J12" s="3" t="n">
-        <v>2004590.969313893</v>
+        <v>1943869.41653763</v>
       </c>
       <c r="K12" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="3" t="n">
-        <v>2004590.969313893</v>
+        <v>1943869.41653763</v>
       </c>
       <c r="M12" s="3" t="n">
-        <v>6347871.402827327</v>
+        <v>6155586.485702494</v>
       </c>
     </row>
     <row r="13">
@@ -2685,37 +2685,37 @@
         <v>14191845.84216233</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>4237135.796223</v>
+        <v>4363427.990487233</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>9954710.045939328</v>
+        <v>9828417.851675095</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>8650527.220454562</v>
+        <v>8395272.682226434</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>250000</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>8400527.220454562</v>
+        <v>8145272.682226434</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>2016126.532909095</v>
+        <v>1954865.443734344</v>
       </c>
       <c r="K13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>2016126.532909095</v>
+        <v>1954865.443734344</v>
       </c>
       <c r="M13" s="3" t="n">
-        <v>6384400.687545467</v>
+        <v>6190407.23849209</v>
       </c>
     </row>
     <row r="14">
@@ -2726,37 +2726,37 @@
         <v>14204902.06979268</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>4328900.972895162</v>
+        <v>4457483.868711052</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>9876001.096897515</v>
+        <v>9747418.201081626</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>8571818.271412749</v>
+        <v>8314273.031632966</v>
       </c>
       <c r="H14" s="3" t="n">
         <v>125000</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>8446818.271412749</v>
+        <v>8189273.031632966</v>
       </c>
       <c r="J14" s="3" t="n">
-        <v>2027236.38513906</v>
+        <v>1965425.527591912</v>
       </c>
       <c r="K14" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>2027236.38513906</v>
+        <v>1965425.527591912</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>6419581.88627369</v>
+        <v>6223847.504041054</v>
       </c>
     </row>
     <row r="15">
@@ -2767,37 +2767,37 @@
         <v>14218213.1110835</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>4422737.067521404</v>
+        <v>4553654.127496649</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>9795476.043562099</v>
+        <v>9664558.983586855</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>8491293.218077336</v>
+        <v>8231413.814138195</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>8491293.218077336</v>
+        <v>8231413.814138195</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>2037910.37233856</v>
+        <v>1975539.315393167</v>
       </c>
       <c r="K15" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>2037910.37233856</v>
+        <v>1975539.315393167</v>
       </c>
       <c r="M15" s="3" t="n">
-        <v>6453382.845738775</v>
+        <v>6255874.498745029</v>
       </c>
     </row>
     <row r="16">
@@ -2808,37 +2808,37 @@
         <v>14231783.9991991</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>4518692.46037346</v>
+        <v>4651987.992853677</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>9713091.538825639</v>
+        <v>9579796.006345421</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G16" s="3" t="n">
-        <v>8408908.713340875</v>
+        <v>8146650.836896761</v>
       </c>
       <c r="H16" s="3" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="3" t="n">
-        <v>8408908.713340875</v>
+        <v>8146650.836896761</v>
       </c>
       <c r="J16" s="3" t="n">
-        <v>2018138.09120181</v>
+        <v>1955196.200855223</v>
       </c>
       <c r="K16" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>2018138.09120181</v>
+        <v>1955196.200855223</v>
       </c>
       <c r="M16" s="3" t="n">
-        <v>6390770.622139065</v>
+        <v>6191454.636041539</v>
       </c>
     </row>
     <row r="17">
@@ -2849,37 +2849,37 @@
         <v>14245619.86733594</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>4616816.698222538</v>
+        <v>4752535.873970879</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>9628803.169113405</v>
+        <v>9493083.993365064</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G17" s="3" t="n">
-        <v>8324620.34362864</v>
+        <v>8059938.823916405</v>
       </c>
       <c r="H17" s="3" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="3" t="n">
-        <v>8324620.34362864</v>
+        <v>8059938.823916405</v>
       </c>
       <c r="J17" s="3" t="n">
-        <v>1997908.882470874</v>
+        <v>1934385.317739937</v>
       </c>
       <c r="K17" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L17" s="3" t="n">
-        <v>1997908.882470874</v>
+        <v>1934385.317739937</v>
       </c>
       <c r="M17" s="3" t="n">
-        <v>6326711.461157767</v>
+        <v>6125553.506176468</v>
       </c>
     </row>
     <row r="18">
@@ -2890,37 +2890,37 @@
         <v>14259725.95071705</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>4717160.523314024</v>
+        <v>4855349.392522041</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>9542565.427403029</v>
+        <v>9404376.558195014</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G18" s="3" t="n">
-        <v>8238382.601918264</v>
+        <v>7971231.388746354</v>
       </c>
       <c r="H18" s="3" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="3" t="n">
-        <v>8238382.601918264</v>
+        <v>7971231.388746354</v>
       </c>
       <c r="J18" s="3" t="n">
-        <v>1977211.824460383</v>
+        <v>1913095.533299125</v>
       </c>
       <c r="K18" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L18" s="3" t="n">
-        <v>1977211.824460383</v>
+        <v>1913095.533299125</v>
       </c>
       <c r="M18" s="3" t="n">
-        <v>6261170.777457881</v>
+        <v>6058135.855447229</v>
       </c>
     </row>
     <row r="19">
@@ -2931,37 +2931,37 @@
         <v>14274107.58862613</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>4819775.903082277</v>
+        <v>4960481.412718607</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>9454331.685543854</v>
+        <v>9313626.175907524</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G19" s="3" t="n">
-        <v>8150148.860059089</v>
+        <v>7880481.006458865</v>
       </c>
       <c r="H19" s="3" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="3" t="n">
-        <v>8150148.860059089</v>
+        <v>7880481.006458865</v>
       </c>
       <c r="J19" s="3" t="n">
-        <v>1956035.726414181</v>
+        <v>1891315.441550127</v>
       </c>
       <c r="K19" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="3" t="n">
-        <v>1956035.726414181</v>
+        <v>1891315.441550127</v>
       </c>
       <c r="M19" s="3" t="n">
-        <v>6194113.133644908</v>
+        <v>5989165.564908737</v>
       </c>
     </row>
     <row r="20">
@@ -2972,37 +2972,37 @@
         <v>14288770.22648234</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>4924716.060624847</v>
+        <v>5067986.072128499</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>9364054.16585749</v>
+        <v>9220784.154353838</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>890000</v>
+        <v>976000</v>
       </c>
       <c r="G20" s="3" t="n">
-        <v>8059871.340372725</v>
+        <v>7787638.984905179</v>
       </c>
       <c r="H20" s="3" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="3" t="n">
-        <v>8059871.340372725</v>
+        <v>7787638.984905179</v>
       </c>
       <c r="J20" s="3" t="n">
-        <v>1934369.121689454</v>
+        <v>1869033.356377243</v>
       </c>
       <c r="K20" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>1934369.121689454</v>
+        <v>1869033.356377243</v>
       </c>
       <c r="M20" s="3" t="n">
-        <v>6125502.218683272</v>
+        <v>5918605.628527936</v>
       </c>
     </row>
   </sheetData>
@@ -3025,9 +3025,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
@@ -3129,13 +3129,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>-19200000</v>
+        <v>-20490000</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>-19200000</v>
+        <v>-20490000</v>
       </c>
       <c r="I2" s="3" t="n">
         <v>12000000</v>
@@ -3147,7 +3147,7 @@
         <v>-600000</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>18600000</v>
+        <v>19890000</v>
       </c>
       <c r="M2" s="3" t="n">
         <v>-600000</v>
@@ -3173,13 +3173,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>-25300000</v>
+        <v>-28310000</v>
       </c>
       <c r="G3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>-25300000</v>
+        <v>-28310000</v>
       </c>
       <c r="I3" s="3" t="n">
         <v>18000000</v>
@@ -3191,7 +3191,7 @@
         <v>-1500000</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>23800000</v>
+        <v>26810000</v>
       </c>
       <c r="M3" s="3" t="n">
         <v>-1500000</v>
@@ -3205,25 +3205,25 @@
         <v>2027</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>5183634.852631579</v>
+        <v>5003923.471219018</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>-1450360.684931507</v>
+        <v>-1443292.191780822</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>6460794.315068493</v>
+        <v>6339722.808219178</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>-0</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>8900000</v>
+        <v>9760000</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>8900000</v>
+        <v>9760000</v>
       </c>
       <c r="I4" s="3" t="n">
         <v>0</v>
@@ -3238,10 +3238,10 @@
         <v>-3875000</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>11485794.31506849</v>
+        <v>12224722.80821918</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>14385794.31506849</v>
+        <v>15124722.80821918</v>
       </c>
     </row>
     <row r="5">
@@ -3249,25 +3249,25 @@
         <v>2028</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>6540707.770231578</v>
+        <v>6359525.788819019</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>-301687.5665753425</v>
+        <v>-301546.1967123288</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>9395089.693424655</v>
+        <v>9265156.063287672</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>-0</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>8900000</v>
+        <v>9760000</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>8900000</v>
+        <v>9760000</v>
       </c>
       <c r="I5" s="3" t="n">
         <v>0</v>
@@ -3282,10 +3282,10 @@
         <v>-3750000</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>14545089.69342466</v>
+        <v>15275156.06328767</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>28930884.00849315</v>
+        <v>30399878.87150685</v>
       </c>
     </row>
     <row r="6">
@@ -3293,16 +3293,16 @@
         <v>2029</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>6957091.673019581</v>
+        <v>6774411.313607019</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>-98308.91295616422</v>
+        <v>-98164.71569589025</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>10146341.90334384</v>
+        <v>10014439.55060411</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>-0</v>
@@ -3326,10 +3326,10 @@
         <v>-3625000</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>6521341.903343838</v>
+        <v>6389439.550604111</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>35452225.91183698</v>
+        <v>36789318.42211096</v>
       </c>
     </row>
     <row r="7">
@@ -3337,16 +3337,16 @@
         <v>2030</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>6906076.13077706</v>
+        <v>6721869.076144498</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>3245.400050712109</v>
+        <v>3392.481256191531</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>10180770.50287371</v>
+        <v>10046862.22457919</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>-0</v>
@@ -3370,10 +3370,10 @@
         <v>-3500000</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>6680770.502873713</v>
+        <v>6546862.224579189</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>42132996.41471069</v>
+        <v>43336180.64669015</v>
       </c>
     </row>
     <row r="8">
@@ -3381,16 +3381,16 @@
         <v>2031</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>6853889.878323385</v>
+        <v>6668127.261409825</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>3320.235319098807</v>
+        <v>3470.258148687892</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>8790936.988603106</v>
+        <v>9675284.946968369</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>-0</v>
@@ -3414,10 +3414,10 @@
         <v>-3375000</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>5415936.988603106</v>
+        <v>6300284.946968369</v>
       </c>
       <c r="N8" s="3" t="n">
-        <v>47548933.4033138</v>
+        <v>49636465.59365851</v>
       </c>
     </row>
     <row r="9">
@@ -3425,16 +3425,16 @@
         <v>2032</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>6800505.113222653</v>
+        <v>6613157.506294307</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>3396.855434792757</v>
+        <v>3549.87872097356</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>8288084.794142212</v>
+        <v>8229852.554463941</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>-0</v>
@@ -3458,10 +3458,10 @@
         <v>-3250000</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>5038084.794142212</v>
+        <v>4979852.554463941</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>52587018.19745601</v>
+        <v>54616318.14812245</v>
       </c>
     </row>
     <row r="10">
@@ -3469,16 +3469,16 @@
         <v>2033</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>6745893.352269918</v>
+        <v>6556930.755873442</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>3475.304642237228</v>
+        <v>3631.388394141657</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>8203551.482396918</v>
+        <v>8143707.313716242</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>-0</v>
@@ -3502,10 +3502,10 @@
         <v>-3125000</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>5078551.482396918</v>
+        <v>5018707.313716242</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>57665569.67985293</v>
+        <v>59635025.46183869</v>
       </c>
     </row>
     <row r="11">
@@ -3513,16 +3513,16 @@
         <v>2034</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>6690025.414345697</v>
+        <v>6499417.246042149</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>3555.628326222242</v>
+        <v>3714.833753164799</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>8117763.868156683</v>
+        <v>8056277.249243975</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>-0</v>
@@ -3546,10 +3546,10 @@
         <v>-3000000</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>5117763.868156683</v>
+        <v>5056277.249243975</v>
       </c>
       <c r="N11" s="3" t="n">
-        <v>62783333.5480096</v>
+        <v>64691302.71108267</v>
       </c>
     </row>
     <row r="12">
@@ -3557,16 +3557,16 @@
         <v>2035</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>6632871.402827327</v>
+        <v>6440586.485702494</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>3637.873042344319</v>
+        <v>3800.262577825662</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>8030692.101354436</v>
+        <v>7967531.91772898</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>-0</v>
@@ -3590,10 +3590,10 @@
         <v>-2875000</v>
       </c>
       <c r="M12" s="3" t="n">
-        <v>5155692.101354436</v>
+        <v>5092531.91772898</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>67939025.64936404</v>
+        <v>69783834.62881164</v>
       </c>
     </row>
     <row r="13">
@@ -3601,16 +3601,16 @@
         <v>2036</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>6574400.687545467</v>
+        <v>6380407.23849209</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>3722.086548307328</v>
+        <v>3887.723874498333</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>7942305.599578538</v>
+        <v>7877440.131815247</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>-0</v>
@@ -3634,10 +3634,10 @@
         <v>-2750000</v>
       </c>
       <c r="M13" s="3" t="n">
-        <v>5192305.599578538</v>
+        <v>5127440.131815247</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>73131331.24894258</v>
+        <v>74911274.76062688</v>
       </c>
     </row>
     <row r="14">
@@ -3645,16 +3645,16 @@
         <v>2037</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>6514581.88627369</v>
+        <v>6318847.504041054</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>3808.317836084403</v>
+        <v>3977.267908799229</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>7852573.029594538</v>
+        <v>7785969.941398514</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>-0</v>
@@ -3678,10 +3678,10 @@
         <v>-2625000</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>5227573.029594538</v>
+        <v>5160969.941398514</v>
       </c>
       <c r="N14" s="3" t="n">
-        <v>78358904.27853712</v>
+        <v>80072244.7020254</v>
       </c>
     </row>
     <row r="15">
@@ -3689,16 +3689,16 @@
         <v>2038</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>6453382.845738775</v>
+        <v>6255874.498745029</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>3896.617164964991</v>
+        <v>4068.946239134122</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>7761462.288388505</v>
+        <v>7693088.614432823</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>-0</v>
@@ -3722,10 +3722,10 @@
         <v>-2500000</v>
       </c>
       <c r="M15" s="3" t="n">
-        <v>5261462.288388505</v>
+        <v>5193088.614432823</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>83620366.56692563</v>
+        <v>85265333.31645823</v>
       </c>
     </row>
     <row r="16">
@@ -3733,16 +3733,16 @@
         <v>2039</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>6390770.622139065</v>
+        <v>6191454.636041539</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>3987.036095519172</v>
+        <v>4162.811751171655</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>7698940.48371935</v>
+        <v>7628762.617241371</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>-0</v>
@@ -3766,10 +3766,10 @@
         <v>0</v>
       </c>
       <c r="M16" s="3" t="n">
-        <v>7698940.48371935</v>
+        <v>7628762.617241371</v>
       </c>
       <c r="N16" s="3" t="n">
-        <v>91319307.05064498</v>
+        <v>92894095.93369959</v>
       </c>
     </row>
     <row r="17">
@@ -3777,16 +3777,16 @@
         <v>2040</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>6326711.461157767</v>
+        <v>6125553.506176468</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>4079.627524492273</v>
+        <v>4258.918693257903</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>7634973.914167025</v>
+        <v>7562957.594318384</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>-0</v>
@@ -3810,10 +3810,10 @@
         <v>0</v>
       </c>
       <c r="M17" s="3" t="n">
-        <v>7634973.914167025</v>
+        <v>7562957.594318384</v>
       </c>
       <c r="N17" s="3" t="n">
-        <v>98954280.96481201</v>
+        <v>100457053.528018</v>
       </c>
     </row>
     <row r="18">
@@ -3821,16 +3821,16 @@
         <v>2041</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>6261170.777457881</v>
+        <v>6058135.855447229</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>4174.445720668009</v>
+        <v>4357.322712808847</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>7569528.048663314</v>
+        <v>7495638.347608697</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>-0</v>
@@ -3854,10 +3854,10 @@
         <v>0</v>
       </c>
       <c r="M18" s="3" t="n">
-        <v>7569528.048663314</v>
+        <v>7495638.347608697</v>
       </c>
       <c r="N18" s="3" t="n">
-        <v>106523809.0134753</v>
+        <v>107952691.8756267</v>
       </c>
     </row>
     <row r="19">
@@ -3865,16 +3865,16 @@
         <v>2042</v>
       </c>
       <c r="B19" s="3" t="n">
-        <v>6194113.133644908</v>
+        <v>5989165.564908737</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>4271.546361724846</v>
+        <v>4458.080893708568</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>7502567.505491397</v>
+        <v>7426768.815251106</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>-0</v>
@@ -3898,10 +3898,10 @@
         <v>0</v>
       </c>
       <c r="M19" s="3" t="n">
-        <v>7502567.505491397</v>
+        <v>7426768.815251106</v>
       </c>
       <c r="N19" s="3" t="n">
-        <v>114026376.5189667</v>
+        <v>115379460.6908778</v>
       </c>
     </row>
     <row r="20">
@@ -3909,16 +3909,16 @@
         <v>2043</v>
       </c>
       <c r="B20" s="3" t="n">
-        <v>6125502.218683272</v>
+        <v>5918605.628527936</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>4370.986572103342</v>
+        <v>4561.251794726646</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>7434056.03074014</v>
+        <v>7356312.049771322</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>-0</v>
@@ -3942,10 +3942,10 @@
         <v>0</v>
       </c>
       <c r="M20" s="3" t="n">
-        <v>7434056.03074014</v>
+        <v>7356312.049771322</v>
       </c>
       <c r="N20" s="3" t="n">
-        <v>121460432.5497069</v>
+        <v>122735772.7406491</v>
       </c>
     </row>
   </sheetData>
@@ -3968,7 +3968,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
@@ -4012,19 +4012,19 @@
         <v>2027</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>6820572.174515235</v>
+        <v>6584109.83055134</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>1450360.684931507</v>
+        <v>1443292.191780822</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>5927456.993184837</v>
+        <v>5969776.448886856</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>2382456.993184837</v>
+        <v>2424776.448886856</v>
       </c>
     </row>
     <row r="3">
@@ -4032,19 +4032,19 @@
         <v>2028</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>8606194.434515234</v>
+        <v>8367797.09055134</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>301687.5665753423</v>
+        <v>301546.1967123288</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>8433203.029141</v>
+        <v>8467124.761555349</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>4983203.029141</v>
+        <v>5017124.761555349</v>
       </c>
     </row>
     <row r="4">
@@ -4052,19 +4052,19 @@
         <v>2029</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>9154067.990815237</v>
+        <v>8913699.096851341</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>98308.91295616422</v>
+        <v>98164.71569589013</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>9052965.585548181</v>
+        <v>9085391.767359789</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>5697965.585548181</v>
+        <v>5730391.767359789</v>
       </c>
     </row>
     <row r="5">
@@ -4072,19 +4072,19 @@
         <v>2030</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>9086942.277338237</v>
+        <v>8844564.573874339</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>-3245.400050712051</v>
+        <v>-3392.481256191386</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>9103504.356312538</v>
+        <v>9134406.726849347</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>5843504.356312538</v>
+        <v>5874406.726849347</v>
       </c>
     </row>
     <row r="6">
@@ -4092,19 +4092,19 @@
         <v>2031</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>9018276.155688666</v>
+        <v>8773851.659749769</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>-3320.235319098691</v>
+        <v>-3470.258148687892</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>9051392.93912725</v>
+        <v>9080742.689007174</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>5886392.93912725</v>
+        <v>5915742.689007174</v>
       </c>
     </row>
     <row r="7">
@@ -4112,19 +4112,19 @@
         <v>2032</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>8948033.043714017</v>
+        <v>8701523.034597773</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>-3396.855434792815</v>
+        <v>-3549.878720973618</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>8998084.794142211</v>
+        <v>9025852.554463942</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>5928084.794142211</v>
+        <v>5955852.554463942</v>
       </c>
     </row>
     <row r="8">
@@ -4132,19 +4132,19 @@
         <v>2033</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>8876175.46351305</v>
+        <v>8627540.468254529</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>-3475.304642237257</v>
+        <v>-3631.388394141803</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>8943551.482396921</v>
+        <v>8969707.313716242</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>5968551.482396921</v>
+        <v>5994707.313716242</v>
       </c>
     </row>
     <row r="9">
@@ -4152,19 +4152,19 @@
         <v>2034</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>8802665.018875916</v>
+        <v>8551864.797423881</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>-3555.628326222301</v>
+        <v>-3714.833753164625</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>8887763.868156683</v>
+        <v>8912277.249243975</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>6007763.868156683</v>
+        <v>6032277.249243975</v>
       </c>
     </row>
     <row r="10">
@@ -4172,19 +4172,19 @@
         <v>2035</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>8727462.37214122</v>
+        <v>8474455.902240124</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>-3637.873042344349</v>
+        <v>-3800.262577825692</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>8830692.101354437</v>
+        <v>8853531.917728981</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>6045692.101354437</v>
+        <v>6068531.917728981</v>
       </c>
     </row>
     <row r="11">
@@ -4192,19 +4192,19 @@
         <v>2036</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>8650527.220454562</v>
+        <v>8395272.682226434</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>-3722.086548307212</v>
+        <v>-3887.723874498392</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>8772305.599578539</v>
+        <v>8793440.131815247</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>6082305.599578539</v>
+        <v>6103440.131815247</v>
       </c>
     </row>
     <row r="12">
@@ -4212,19 +4212,19 @@
         <v>2037</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>8571818.271412749</v>
+        <v>8314273.031632966</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>-3808.317836084403</v>
+        <v>-3977.267908799229</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>8712573.029594537</v>
+        <v>8731969.941398513</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>6117573.029594537</v>
+        <v>6136969.941398513</v>
       </c>
     </row>
     <row r="13">
@@ -4232,19 +4232,19 @@
         <v>2038</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>8491293.218077336</v>
+        <v>8231413.814138195</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>-3896.61716496502</v>
+        <v>-4068.946239134064</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>8651462.288388506</v>
+        <v>8669088.614432823</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>6151462.288388506</v>
+        <v>6169088.614432823</v>
       </c>
     </row>
     <row r="14">
@@ -4252,19 +4252,19 @@
         <v>2039</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>8408908.713340875</v>
+        <v>8146650.836896761</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>-3987.036095519084</v>
+        <v>-4162.811751171714</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>8588940.483719349</v>
+        <v>8604762.617241371</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>8588940.483719349</v>
+        <v>8604762.617241371</v>
       </c>
     </row>
     <row r="15">
@@ -4272,19 +4272,19 @@
         <v>2040</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>8324620.34362864</v>
+        <v>8059938.823916405</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>-4079.627524492331</v>
+        <v>-4258.918693257961</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>8524973.914167024</v>
+        <v>8538957.594318384</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>8524973.914167024</v>
+        <v>8538957.594318384</v>
       </c>
     </row>
     <row r="16">
@@ -4292,19 +4292,19 @@
         <v>2041</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>8238382.601918264</v>
+        <v>7971231.388746354</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>-4174.445720667951</v>
+        <v>-4357.322712808847</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>8459528.048663314</v>
+        <v>8471638.347608697</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>8459528.048663314</v>
+        <v>8471638.347608697</v>
       </c>
     </row>
     <row r="17">
@@ -4312,19 +4312,19 @@
         <v>2042</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>8150148.860059089</v>
+        <v>7880481.006458865</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>-4271.546361724846</v>
+        <v>-4458.080893708393</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>8392567.505491398</v>
+        <v>8402768.815251106</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>8392567.505491398</v>
+        <v>8402768.815251106</v>
       </c>
     </row>
     <row r="18">
@@ -4332,19 +4332,19 @@
         <v>2043</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>8059871.340372725</v>
+        <v>7787638.984905179</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>2194182.825484765</v>
+        <v>2409145.16944866</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>-4370.986572103575</v>
+        <v>-4561.251794726821</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>8324056.03074014</v>
+        <v>8332312.049771322</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>8324056.03074014</v>
+        <v>8332312.049771322</v>
       </c>
     </row>
   </sheetData>
@@ -4399,7 +4399,7 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>75349751.55668171</v>
+        <v>75617284.59900604</v>
       </c>
     </row>
     <row r="4">
@@ -4409,7 +4409,7 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>92489511.45266822</v>
+        <v>92581244.99745914</v>
       </c>
     </row>
     <row r="5">
@@ -4419,7 +4419,7 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>21371845.22870355</v>
+        <v>21393042.3903142</v>
       </c>
     </row>
     <row r="6">
@@ -4429,7 +4429,7 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>96721596.78538527</v>
+        <v>97010326.98932025</v>
       </c>
     </row>
     <row r="7">
@@ -4469,7 +4469,7 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>71721596.78538527</v>
+        <v>72010326.98932025</v>
       </c>
     </row>
     <row r="11">
@@ -4479,7 +4479,7 @@
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>71554994.31900613</v>
+        <v>71803116.34476006</v>
       </c>
     </row>
     <row r="12">
@@ -4489,7 +4489,7 @@
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>166602.4663791358</v>
+        <v>207210.6445601881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>